<commit_message>
update values in excel spreadsheet
</commit_message>
<xml_diff>
--- a/Percent_Ana/DISCus_percent_ana_NEW_05082015.xlsx
+++ b/Percent_Ana/DISCus_percent_ana_NEW_05082015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="-6700" windowWidth="21940" windowHeight="18860" tabRatio="500"/>
+    <workbookView xWindow="27400" yWindow="-6680" windowWidth="21940" windowHeight="18860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Percentage analysis DISCus NEW (5/8/15)</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>375 (21)</t>
+  </si>
+  <si>
+    <t>Difference to predicted</t>
   </si>
 </sst>
 </file>
@@ -246,7 +249,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -262,8 +265,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -277,8 +282,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -286,6 +294,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -293,6 +302,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1087,7 +1097,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="45">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1097,6 +1107,9 @@
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
+      <c r="H26" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="10" t="s">
@@ -1145,6 +1158,9 @@
         <f>100-F28</f>
         <v>1.3630731102850007</v>
       </c>
+      <c r="H28">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
@@ -1170,6 +1186,9 @@
         <f>100-F29</f>
         <v>19.013237063778575</v>
       </c>
+      <c r="H29">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
@@ -1195,6 +1214,9 @@
         <f t="shared" ref="G30:G32" si="4">100-F30</f>
         <v>36.440677966101696</v>
       </c>
+      <c r="H30" s="12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
@@ -1220,6 +1242,9 @@
         <f t="shared" si="4"/>
         <v>52.873563218390807</v>
       </c>
+      <c r="H31" s="12">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
@@ -1245,8 +1270,11 @@
         <f t="shared" si="4"/>
         <v>74.462365591397855</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1270,10 +1298,43 @@
         <f>100-F33</f>
         <v>90.736040609137063</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="B34">
+        <f>(27+19+18+12+10+8)/6</f>
+        <v>15.666666666666666</v>
+      </c>
+      <c r="C34">
+        <f>(31+29+21+19+14+11)/6</f>
+        <v>20.833333333333332</v>
+      </c>
+      <c r="D34">
+        <f>(4+9+14+17+23+28)/6</f>
+        <v>15.833333333333334</v>
+      </c>
+      <c r="E34">
+        <f>(3+7+10+12+15+21)/6</f>
+        <v>11.333333333333334</v>
+      </c>
+      <c r="H34">
+        <f>AVERAGE(H28:H33)</f>
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35">
+        <f>AVERAGE(B34:C34)</f>
+        <v>18.25</v>
+      </c>
+      <c r="D35">
+        <f>AVERAGE(D34:E34)</f>
+        <v>13.583333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>